<commit_message>
ok for visu, now methodo
</commit_message>
<xml_diff>
--- a/Risk Assessment/data/VNM_1_statistic.xlsx
+++ b/Risk Assessment/data/VNM_1_statistic.xlsx
@@ -13,11 +13,11 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1586665606" val="973" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1586665606" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1586665606"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1586665606"/>
-      <pm:sortOptions xmlns:pm="smNativeData" id="1586665606">
+      <pm:revision xmlns:pm="smNativeData" day="1586694348" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1586694348" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1586694348" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1586694348"/>
+      <pm:sortOptions xmlns:pm="smNativeData" id="1586694348">
         <pm:column colId="3"/>
         <pm:column colId="-1"/>
         <pm:column colId="-1"/>
@@ -269,7 +269,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="11">
+  <numFmts count="9">
     <numFmt numFmtId="5" formatCode="#,##0\ &quot;$&quot;;\-#,##0\ &quot;$&quot;"/>
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;$&quot;;[Red]\-#,##0\ &quot;$&quot;"/>
     <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;$&quot;;\-#,##0.00\ &quot;$&quot;"/>
@@ -278,9 +278,7 @@
     <numFmt numFmtId="41" formatCode="_-* #,##0\ _$_-;\-* #,##0\ _$_-;_-* &quot;-&quot;\ _$_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="165" formatCode="MM/DD/YYYY;@"/>
-    <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD;@"/>
+    <numFmt numFmtId="164" formatCode="YYYY\-MM\-DD;@"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -290,7 +288,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1586665606" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1586694348" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -312,7 +310,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1586665606" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586694348" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -334,7 +332,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1586665606"/>
+          <pm:border xmlns:pm="smNativeData" id="1586694348"/>
         </ext>
       </extLst>
     </border>
@@ -353,7 +351,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1586665606"/>
+          <pm:border xmlns:pm="smNativeData" id="1586694348"/>
         </ext>
       </extLst>
     </border>
@@ -361,10 +359,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -372,7 +369,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1586665606" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1586694348" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -636,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L243"/>
+  <dimension ref="A1:F243"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="D239" sqref="D239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -677,7 +674,7 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="1" t="n">
         <v>43892</v>
       </c>
       <c r="E2" t="s">
@@ -697,7 +694,7 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="1" t="n">
         <v>43892</v>
       </c>
       <c r="E3" t="s">
@@ -717,7 +714,7 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="1" t="n">
         <v>43892</v>
       </c>
       <c r="E4" t="s">
@@ -737,7 +734,7 @@
       <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="1" t="n">
         <v>43892</v>
       </c>
       <c r="E5" t="s">
@@ -747,7 +744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:4">
       <c r="A6" t="n">
         <v>22</v>
       </c>
@@ -757,7 +754,7 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -771,7 +768,7 @@
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -785,7 +782,7 @@
       <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -799,7 +796,7 @@
       <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -813,7 +810,7 @@
       <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -827,7 +824,7 @@
       <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -841,7 +838,7 @@
       <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -855,7 +852,7 @@
       <c r="C13" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D13" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -869,7 +866,7 @@
       <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="D14" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -883,7 +880,7 @@
       <c r="C15" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="D15" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -897,7 +894,7 @@
       <c r="C16" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="2" t="n">
+      <c r="D16" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -911,7 +908,7 @@
       <c r="C17" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="2" t="n">
+      <c r="D17" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -925,7 +922,7 @@
       <c r="C18" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="2" t="n">
+      <c r="D18" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -939,7 +936,7 @@
       <c r="C19" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="2" t="n">
+      <c r="D19" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -953,7 +950,7 @@
       <c r="C20" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="2" t="n">
+      <c r="D20" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -967,7 +964,7 @@
       <c r="C21" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="2" t="n">
+      <c r="D21" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -981,11 +978,11 @@
       <c r="C22" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="2" t="n">
+      <c r="D22" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:4">
       <c r="A23" t="n">
         <v>42</v>
       </c>
@@ -995,11 +992,11 @@
       <c r="C23" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="2" t="n">
+      <c r="D23" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:4">
       <c r="A24" t="n">
         <v>43</v>
       </c>
@@ -1009,7 +1006,7 @@
       <c r="C24" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="2" t="n">
+      <c r="D24" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -1023,7 +1020,7 @@
       <c r="C25" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="2" t="n">
+      <c r="D25" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -1037,7 +1034,7 @@
       <c r="C26" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="2" t="n">
+      <c r="D26" s="1" t="n">
         <v>43892</v>
       </c>
       <c r="E26" t="s">
@@ -1047,7 +1044,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:4">
       <c r="A27" t="n">
         <v>48</v>
       </c>
@@ -1057,7 +1054,7 @@
       <c r="C27" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="2" t="n">
+      <c r="D27" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -1071,7 +1068,7 @@
       <c r="C28" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="2" t="n">
+      <c r="D28" s="1" t="n">
         <v>43892</v>
       </c>
     </row>
@@ -1085,7 +1082,7 @@
       <c r="C29" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="2" t="n">
+      <c r="D29" s="1" t="n">
         <v>43892</v>
       </c>
       <c r="E29" t="s">
@@ -1095,7 +1092,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:4">
       <c r="A30" t="n">
         <v>45</v>
       </c>
@@ -1105,11 +1102,11 @@
       <c r="C30" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="2" t="n">
+      <c r="D30" s="1" t="n">
         <v>43893</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:4">
       <c r="A31" t="n">
         <v>100</v>
       </c>
@@ -1119,11 +1116,11 @@
       <c r="C31" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="2" t="n">
+      <c r="D31" s="1" t="n">
         <v>43893</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:4">
       <c r="A32" t="n">
         <v>18</v>
       </c>
@@ -1133,7 +1130,7 @@
       <c r="C32" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="2" t="n">
+      <c r="D32" s="1" t="n">
         <v>43894</v>
       </c>
     </row>
@@ -1147,11 +1144,11 @@
       <c r="C33" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="2" t="n">
+      <c r="D33" s="1" t="n">
         <v>43894</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:5">
       <c r="A34" t="n">
         <v>39</v>
       </c>
@@ -1161,14 +1158,14 @@
       <c r="C34" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="2" t="n">
+      <c r="D34" s="1" t="n">
         <v>43894</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:4">
       <c r="A35" t="n">
         <v>61</v>
       </c>
@@ -1178,11 +1175,11 @@
       <c r="C35" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="2" t="n">
+      <c r="D35" s="1" t="n">
         <v>43894</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:4">
       <c r="A36" t="n">
         <v>67</v>
       </c>
@@ -1192,7 +1189,7 @@
       <c r="C36" t="s">
         <v>20</v>
       </c>
-      <c r="D36" s="2" t="n">
+      <c r="D36" s="1" t="n">
         <v>43894</v>
       </c>
     </row>
@@ -1206,7 +1203,7 @@
       <c r="C37" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="2" t="n">
+      <c r="D37" s="1" t="n">
         <v>43896</v>
       </c>
     </row>
@@ -1220,14 +1217,14 @@
       <c r="C38" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="2" t="n">
+      <c r="D38" s="1" t="n">
         <v>43896</v>
       </c>
       <c r="E38" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:4">
       <c r="A39" t="n">
         <v>65</v>
       </c>
@@ -1237,7 +1234,7 @@
       <c r="C39" t="s">
         <v>15</v>
       </c>
-      <c r="D39" s="2" t="n">
+      <c r="D39" s="1" t="n">
         <v>43897</v>
       </c>
     </row>
@@ -1251,14 +1248,14 @@
       <c r="C40" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="2" t="n">
+      <c r="D40" s="1" t="n">
         <v>43897</v>
       </c>
       <c r="E40" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:4">
       <c r="A41" t="n">
         <v>54</v>
       </c>
@@ -1268,11 +1265,11 @@
       <c r="C41" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="2" t="n">
+      <c r="D41" s="1" t="n">
         <v>43898</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:4">
       <c r="A42" t="n">
         <v>91</v>
       </c>
@@ -1282,11 +1279,11 @@
       <c r="C42" t="s">
         <v>15</v>
       </c>
-      <c r="D42" s="2" t="n">
+      <c r="D42" s="1" t="n">
         <v>43898</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:4">
       <c r="A43" t="n">
         <v>32</v>
       </c>
@@ -1296,7 +1293,7 @@
       <c r="C43" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="2" t="n">
+      <c r="D43" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
@@ -1310,7 +1307,7 @@
       <c r="C44" t="s">
         <v>6</v>
       </c>
-      <c r="D44" s="2" t="n">
+      <c r="D44" s="1" t="n">
         <v>43899</v>
       </c>
       <c r="E44" t="s">
@@ -1330,7 +1327,7 @@
       <c r="C45" t="s">
         <v>6</v>
       </c>
-      <c r="D45" s="2" t="n">
+      <c r="D45" s="1" t="n">
         <v>43899</v>
       </c>
       <c r="E45" t="s">
@@ -1340,7 +1337,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:4">
       <c r="A46" t="n">
         <v>52</v>
       </c>
@@ -1350,11 +1347,11 @@
       <c r="C46" t="s">
         <v>9</v>
       </c>
-      <c r="D46" s="2" t="n">
+      <c r="D46" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:4">
       <c r="A47" t="n">
         <v>57</v>
       </c>
@@ -1364,11 +1361,11 @@
       <c r="C47" t="s">
         <v>13</v>
       </c>
-      <c r="D47" s="2" t="n">
+      <c r="D47" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:4">
       <c r="A48" t="n">
         <v>60</v>
       </c>
@@ -1378,7 +1375,7 @@
       <c r="C48" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="2" t="n">
+      <c r="D48" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
@@ -1392,7 +1389,7 @@
       <c r="C49" t="s">
         <v>6</v>
       </c>
-      <c r="D49" s="2" t="n">
+      <c r="D49" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
@@ -1406,7 +1403,7 @@
       <c r="C50" t="s">
         <v>26</v>
       </c>
-      <c r="D50" s="2" t="n">
+      <c r="D50" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
@@ -1420,7 +1417,7 @@
       <c r="C51" t="s">
         <v>6</v>
       </c>
-      <c r="D51" s="2" t="n">
+      <c r="D51" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
@@ -1434,11 +1431,11 @@
       <c r="C52" t="s">
         <v>6</v>
       </c>
-      <c r="D52" s="2" t="n">
+      <c r="D52" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:4">
       <c r="A53" t="n">
         <v>169</v>
       </c>
@@ -1448,11 +1445,11 @@
       <c r="C53" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="2" t="n">
+      <c r="D53" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:4">
       <c r="A54" t="n">
         <v>174</v>
       </c>
@@ -1462,11 +1459,11 @@
       <c r="C54" t="s">
         <v>6</v>
       </c>
-      <c r="D54" s="2" t="n">
+      <c r="D54" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:4">
       <c r="A55" t="n">
         <v>175</v>
       </c>
@@ -1476,11 +1473,11 @@
       <c r="C55" t="s">
         <v>6</v>
       </c>
-      <c r="D55" s="2" t="n">
+      <c r="D55" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:4">
       <c r="A56" t="n">
         <v>176</v>
       </c>
@@ -1490,7 +1487,7 @@
       <c r="C56" t="s">
         <v>6</v>
       </c>
-      <c r="D56" s="2" t="n">
+      <c r="D56" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
@@ -1504,7 +1501,7 @@
       <c r="C57" t="s">
         <v>6</v>
       </c>
-      <c r="D57" s="2" t="n">
+      <c r="D57" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
@@ -1518,7 +1515,7 @@
       <c r="C58" t="s">
         <v>27</v>
       </c>
-      <c r="D58" s="2" t="n">
+      <c r="D58" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
@@ -1532,14 +1529,14 @@
       <c r="C59" t="s">
         <v>6</v>
       </c>
-      <c r="D59" s="2" t="n">
+      <c r="D59" s="1" t="n">
         <v>43899</v>
       </c>
       <c r="E59" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:4">
       <c r="A60" t="n">
         <v>188</v>
       </c>
@@ -1549,7 +1546,7 @@
       <c r="C60" t="s">
         <v>6</v>
       </c>
-      <c r="D60" s="2" t="n">
+      <c r="D60" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
@@ -1563,14 +1560,14 @@
       <c r="C61" t="s">
         <v>6</v>
       </c>
-      <c r="D61" s="2" t="n">
+      <c r="D61" s="1" t="n">
         <v>43899</v>
       </c>
       <c r="E61" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:4">
       <c r="A62" t="n">
         <v>190</v>
       </c>
@@ -1580,11 +1577,11 @@
       <c r="C62" t="s">
         <v>6</v>
       </c>
-      <c r="D62" s="2" t="n">
+      <c r="D62" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:4">
       <c r="A63" t="n">
         <v>191</v>
       </c>
@@ -1594,7 +1591,7 @@
       <c r="C63" t="s">
         <v>6</v>
       </c>
-      <c r="D63" s="2" t="n">
+      <c r="D63" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
@@ -1608,7 +1605,7 @@
       <c r="C64" t="s">
         <v>6</v>
       </c>
-      <c r="D64" s="2" t="n">
+      <c r="D64" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
@@ -1622,7 +1619,7 @@
       <c r="C65" t="s">
         <v>6</v>
       </c>
-      <c r="D65" s="2" t="n">
+      <c r="D65" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
@@ -1636,7 +1633,7 @@
       <c r="C66" t="s">
         <v>6</v>
       </c>
-      <c r="D66" s="2" t="n">
+      <c r="D66" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
@@ -1650,11 +1647,11 @@
       <c r="C67" t="s">
         <v>6</v>
       </c>
-      <c r="D67" s="2" t="n">
+      <c r="D67" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:4">
       <c r="A68" t="n">
         <v>196</v>
       </c>
@@ -1664,11 +1661,11 @@
       <c r="C68" t="s">
         <v>6</v>
       </c>
-      <c r="D68" s="2" t="n">
+      <c r="D68" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:4">
       <c r="A69" t="n">
         <v>198</v>
       </c>
@@ -1678,11 +1675,11 @@
       <c r="C69" t="s">
         <v>6</v>
       </c>
-      <c r="D69" s="2" t="n">
+      <c r="D69" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:4">
       <c r="A70" t="n">
         <v>199</v>
       </c>
@@ -1692,11 +1689,11 @@
       <c r="C70" t="s">
         <v>6</v>
       </c>
-      <c r="D70" s="2" t="n">
+      <c r="D70" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:4">
       <c r="A71" t="n">
         <v>200</v>
       </c>
@@ -1706,11 +1703,11 @@
       <c r="C71" t="s">
         <v>6</v>
       </c>
-      <c r="D71" s="2" t="n">
+      <c r="D71" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:4">
       <c r="A72" t="n">
         <v>201</v>
       </c>
@@ -1720,11 +1717,11 @@
       <c r="C72" t="s">
         <v>6</v>
       </c>
-      <c r="D72" s="2" t="n">
+      <c r="D72" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:4">
       <c r="A73" t="n">
         <v>202</v>
       </c>
@@ -1734,7 +1731,7 @@
       <c r="C73" t="s">
         <v>6</v>
       </c>
-      <c r="D73" s="2" t="n">
+      <c r="D73" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
@@ -1748,7 +1745,7 @@
       <c r="C74" t="s">
         <v>6</v>
       </c>
-      <c r="D74" s="2" t="n">
+      <c r="D74" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
@@ -1762,7 +1759,7 @@
       <c r="C75" t="s">
         <v>6</v>
       </c>
-      <c r="D75" s="2" t="n">
+      <c r="D75" s="1" t="n">
         <v>43899</v>
       </c>
     </row>
@@ -1776,7 +1773,7 @@
       <c r="C76" t="s">
         <v>6</v>
       </c>
-      <c r="D76" s="2" t="n">
+      <c r="D76" s="1" t="n">
         <v>43899</v>
       </c>
       <c r="E76" t="s">
@@ -1793,14 +1790,14 @@
       <c r="C77" t="s">
         <v>6</v>
       </c>
-      <c r="D77" s="2" t="n">
+      <c r="D77" s="1" t="n">
         <v>43899</v>
       </c>
       <c r="E77" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:12">
+    <row r="78" spans="1:4">
       <c r="A78" t="n">
         <v>53</v>
       </c>
@@ -1810,7 +1807,7 @@
       <c r="C78" t="s">
         <v>15</v>
       </c>
-      <c r="D78" s="2" t="n">
+      <c r="D78" s="1" t="n">
         <v>43900</v>
       </c>
     </row>
@@ -1824,7 +1821,7 @@
       <c r="C79" t="s">
         <v>6</v>
       </c>
-      <c r="D79" s="2" t="n">
+      <c r="D79" s="1" t="n">
         <v>43900</v>
       </c>
     </row>
@@ -1838,7 +1835,7 @@
       <c r="C80" t="s">
         <v>28</v>
       </c>
-      <c r="D80" s="2" t="n">
+      <c r="D80" s="1" t="n">
         <v>43900</v>
       </c>
     </row>
@@ -1852,7 +1849,7 @@
       <c r="C81" t="s">
         <v>15</v>
       </c>
-      <c r="D81" s="2" t="n">
+      <c r="D81" s="1" t="n">
         <v>43900</v>
       </c>
     </row>
@@ -1866,7 +1863,7 @@
       <c r="C82" t="s">
         <v>28</v>
       </c>
-      <c r="D82" s="2" t="n">
+      <c r="D82" s="1" t="n">
         <v>43900</v>
       </c>
     </row>
@@ -1880,7 +1877,7 @@
       <c r="C83" t="s">
         <v>6</v>
       </c>
-      <c r="D83" s="2" t="n">
+      <c r="D83" s="1" t="n">
         <v>43901</v>
       </c>
     </row>
@@ -1894,7 +1891,7 @@
       <c r="C84" t="s">
         <v>29</v>
       </c>
-      <c r="D84" s="2" t="n">
+      <c r="D84" s="1" t="n">
         <v>43901</v>
       </c>
     </row>
@@ -1908,7 +1905,7 @@
       <c r="C85" t="s">
         <v>6</v>
       </c>
-      <c r="D85" s="2" t="n">
+      <c r="D85" s="1" t="n">
         <v>43902</v>
       </c>
       <c r="E85" t="s">
@@ -1928,7 +1925,7 @@
       <c r="C86" t="s">
         <v>6</v>
       </c>
-      <c r="D86" s="2" t="n">
+      <c r="D86" s="1" t="n">
         <v>43902</v>
       </c>
       <c r="E86" t="s">
@@ -1938,7 +1935,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="87" spans="1:12">
+    <row r="87" spans="1:4">
       <c r="A87" t="n">
         <v>148</v>
       </c>
@@ -1948,7 +1945,7 @@
       <c r="C87" t="s">
         <v>6</v>
       </c>
-      <c r="D87" s="2" t="n">
+      <c r="D87" s="1" t="n">
         <v>43902</v>
       </c>
     </row>
@@ -1962,7 +1959,7 @@
       <c r="C88" t="s">
         <v>6</v>
       </c>
-      <c r="D88" s="2" t="n">
+      <c r="D88" s="1" t="n">
         <v>43902</v>
       </c>
     </row>
@@ -1976,11 +1973,11 @@
       <c r="C89" t="s">
         <v>6</v>
       </c>
-      <c r="D89" s="2" t="n">
+      <c r="D89" s="1" t="n">
         <v>43902</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:5">
       <c r="A90" t="n">
         <v>213</v>
       </c>
@@ -1990,14 +1987,14 @@
       <c r="C90" t="s">
         <v>6</v>
       </c>
-      <c r="D90" s="2" t="n">
+      <c r="D90" s="1" t="n">
         <v>43902</v>
       </c>
       <c r="E90" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:4">
       <c r="A91" t="n">
         <v>243</v>
       </c>
@@ -2007,11 +2004,11 @@
       <c r="C91" t="s">
         <v>6</v>
       </c>
-      <c r="D91" s="2" t="n">
+      <c r="D91" s="1" t="n">
         <v>43902</v>
       </c>
     </row>
-    <row r="92" spans="1:12">
+    <row r="92" spans="1:5">
       <c r="A92" t="n">
         <v>69</v>
       </c>
@@ -2021,14 +2018,14 @@
       <c r="C92" t="s">
         <v>6</v>
       </c>
-      <c r="D92" s="2" t="n">
+      <c r="D92" s="1" t="n">
         <v>43903</v>
       </c>
       <c r="E92" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="93" spans="1:12">
+    <row r="93" spans="1:4">
       <c r="A93" t="n">
         <v>150</v>
       </c>
@@ -2038,11 +2035,11 @@
       <c r="C93" t="s">
         <v>15</v>
       </c>
-      <c r="D93" s="2" t="n">
+      <c r="D93" s="1" t="n">
         <v>43903</v>
       </c>
     </row>
-    <row r="94" spans="1:12">
+    <row r="94" spans="1:4">
       <c r="A94" t="n">
         <v>187</v>
       </c>
@@ -2052,11 +2049,11 @@
       <c r="C94" t="s">
         <v>6</v>
       </c>
-      <c r="D94" s="2" t="n">
+      <c r="D94" s="1" t="n">
         <v>43903</v>
       </c>
     </row>
-    <row r="95" spans="1:12">
+    <row r="95" spans="1:4">
       <c r="A95" t="n">
         <v>55</v>
       </c>
@@ -2066,11 +2063,11 @@
       <c r="C95" t="s">
         <v>6</v>
       </c>
-      <c r="D95" s="2" t="n">
+      <c r="D95" s="1" t="n">
         <v>43904</v>
       </c>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:4">
       <c r="A96" t="n">
         <v>68</v>
       </c>
@@ -2080,11 +2077,11 @@
       <c r="C96" t="s">
         <v>11</v>
       </c>
-      <c r="D96" s="2" t="n">
+      <c r="D96" s="1" t="n">
         <v>43904</v>
       </c>
     </row>
-    <row r="97" spans="1:12">
+    <row r="97" spans="1:4">
       <c r="A97" t="n">
         <v>97</v>
       </c>
@@ -2094,11 +2091,11 @@
       <c r="C97" t="s">
         <v>15</v>
       </c>
-      <c r="D97" s="2" t="n">
+      <c r="D97" s="1" t="n">
         <v>43904</v>
       </c>
     </row>
-    <row r="98" spans="1:12">
+    <row r="98" spans="1:4">
       <c r="A98" t="n">
         <v>98</v>
       </c>
@@ -2108,11 +2105,11 @@
       <c r="C98" t="s">
         <v>15</v>
       </c>
-      <c r="D98" s="2" t="n">
+      <c r="D98" s="1" t="n">
         <v>43904</v>
       </c>
     </row>
-    <row r="99" spans="1:12">
+    <row r="99" spans="1:4">
       <c r="A99" t="n">
         <v>120</v>
       </c>
@@ -2122,11 +2119,11 @@
       <c r="C99" t="s">
         <v>15</v>
       </c>
-      <c r="D99" s="2" t="n">
+      <c r="D99" s="1" t="n">
         <v>43904</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:4">
       <c r="A100" t="n">
         <v>124</v>
       </c>
@@ -2136,11 +2133,11 @@
       <c r="C100" t="s">
         <v>15</v>
       </c>
-      <c r="D100" s="2" t="n">
+      <c r="D100" s="1" t="n">
         <v>43904</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:4">
       <c r="A101" t="n">
         <v>125</v>
       </c>
@@ -2150,11 +2147,11 @@
       <c r="C101" t="s">
         <v>15</v>
       </c>
-      <c r="D101" s="2" t="n">
+      <c r="D101" s="1" t="n">
         <v>43904</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:4">
       <c r="A102" t="n">
         <v>126</v>
       </c>
@@ -2164,7 +2161,7 @@
       <c r="C102" t="s">
         <v>15</v>
       </c>
-      <c r="D102" s="2" t="n">
+      <c r="D102" s="1" t="n">
         <v>43904</v>
       </c>
     </row>
@@ -2178,7 +2175,7 @@
       <c r="C103" t="s">
         <v>15</v>
       </c>
-      <c r="D103" s="2" t="n">
+      <c r="D103" s="1" t="n">
         <v>43904</v>
       </c>
     </row>
@@ -2192,7 +2189,7 @@
       <c r="C104" t="s">
         <v>15</v>
       </c>
-      <c r="D104" s="2" t="n">
+      <c r="D104" s="1" t="n">
         <v>43904</v>
       </c>
     </row>
@@ -2206,7 +2203,7 @@
       <c r="C105" t="s">
         <v>15</v>
       </c>
-      <c r="D105" s="2" t="n">
+      <c r="D105" s="1" t="n">
         <v>43904</v>
       </c>
     </row>
@@ -2220,7 +2217,7 @@
       <c r="C106" t="s">
         <v>15</v>
       </c>
-      <c r="D106" s="2" t="n">
+      <c r="D106" s="1" t="n">
         <v>43904</v>
       </c>
     </row>
@@ -2234,7 +2231,7 @@
       <c r="C107" t="s">
         <v>15</v>
       </c>
-      <c r="D107" s="2" t="n">
+      <c r="D107" s="1" t="n">
         <v>43904</v>
       </c>
     </row>
@@ -2248,7 +2245,7 @@
       <c r="C108" t="s">
         <v>15</v>
       </c>
-      <c r="D108" s="2" t="n">
+      <c r="D108" s="1" t="n">
         <v>43904</v>
       </c>
     </row>
@@ -2262,7 +2259,7 @@
       <c r="C109" t="s">
         <v>15</v>
       </c>
-      <c r="D109" s="2" t="n">
+      <c r="D109" s="1" t="n">
         <v>43904</v>
       </c>
     </row>
@@ -2276,7 +2273,7 @@
       <c r="C110" t="s">
         <v>6</v>
       </c>
-      <c r="D110" s="2" t="n">
+      <c r="D110" s="1" t="n">
         <v>43905</v>
       </c>
       <c r="E110" t="s">
@@ -2296,7 +2293,7 @@
       <c r="C111" t="s">
         <v>6</v>
       </c>
-      <c r="D111" s="2" t="n">
+      <c r="D111" s="1" t="n">
         <v>43905</v>
       </c>
       <c r="E111" t="s">
@@ -2306,7 +2303,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:4">
       <c r="A112" t="n">
         <v>75</v>
       </c>
@@ -2316,11 +2313,11 @@
       <c r="C112" t="s">
         <v>15</v>
       </c>
-      <c r="D112" s="2" t="n">
+      <c r="D112" s="1" t="n">
         <v>43905</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:4">
       <c r="A113" t="n">
         <v>79</v>
       </c>
@@ -2330,11 +2327,11 @@
       <c r="C113" t="s">
         <v>38</v>
       </c>
-      <c r="D113" s="2" t="n">
+      <c r="D113" s="1" t="n">
         <v>43905</v>
       </c>
     </row>
-    <row r="114" spans="1:12">
+    <row r="114" spans="1:4">
       <c r="A114" t="n">
         <v>80</v>
       </c>
@@ -2344,7 +2341,7 @@
       <c r="C114" t="s">
         <v>38</v>
       </c>
-      <c r="D114" s="2" t="n">
+      <c r="D114" s="1" t="n">
         <v>43905</v>
       </c>
     </row>
@@ -2358,11 +2355,11 @@
       <c r="C115" t="s">
         <v>39</v>
       </c>
-      <c r="D115" s="2" t="n">
+      <c r="D115" s="1" t="n">
         <v>43905</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:4">
       <c r="A116" t="n">
         <v>82</v>
       </c>
@@ -2372,11 +2369,11 @@
       <c r="C116" t="s">
         <v>15</v>
       </c>
-      <c r="D116" s="2" t="n">
+      <c r="D116" s="1" t="n">
         <v>43905</v>
       </c>
     </row>
-    <row r="117" spans="1:12">
+    <row r="117" spans="1:4">
       <c r="A117" t="n">
         <v>83</v>
       </c>
@@ -2386,7 +2383,7 @@
       <c r="C117" t="s">
         <v>15</v>
       </c>
-      <c r="D117" s="2" t="n">
+      <c r="D117" s="1" t="n">
         <v>43905</v>
       </c>
     </row>
@@ -2400,14 +2397,14 @@
       <c r="C118" t="s">
         <v>23</v>
       </c>
-      <c r="D118" s="2" t="n">
+      <c r="D118" s="1" t="n">
         <v>43905</v>
       </c>
       <c r="E118" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="119" spans="1:12">
+    <row r="119" spans="1:5">
       <c r="A119" t="n">
         <v>114</v>
       </c>
@@ -2417,14 +2414,14 @@
       <c r="C119" t="s">
         <v>23</v>
       </c>
-      <c r="D119" s="2" t="n">
+      <c r="D119" s="1" t="n">
         <v>43905</v>
       </c>
       <c r="E119" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:4">
       <c r="A120" t="n">
         <v>119</v>
       </c>
@@ -2434,11 +2431,11 @@
       <c r="C120" t="s">
         <v>15</v>
       </c>
-      <c r="D120" s="2" t="n">
+      <c r="D120" s="1" t="n">
         <v>43905</v>
       </c>
     </row>
-    <row r="121" spans="1:12">
+    <row r="121" spans="1:4">
       <c r="A121" t="n">
         <v>137</v>
       </c>
@@ -2448,11 +2445,11 @@
       <c r="C121" t="s">
         <v>23</v>
       </c>
-      <c r="D121" s="2" t="n">
+      <c r="D121" s="1" t="n">
         <v>43905</v>
       </c>
     </row>
-    <row r="122" spans="1:11">
+    <row r="122" spans="1:4">
       <c r="A122" t="n">
         <v>151</v>
       </c>
@@ -2462,11 +2459,11 @@
       <c r="C122" t="s">
         <v>15</v>
       </c>
-      <c r="D122" s="2" t="n">
+      <c r="D122" s="1" t="n">
         <v>43905</v>
       </c>
     </row>
-    <row r="123" spans="1:12">
+    <row r="123" spans="1:4">
       <c r="A123" t="n">
         <v>152</v>
       </c>
@@ -2476,11 +2473,11 @@
       <c r="C123" t="s">
         <v>15</v>
       </c>
-      <c r="D123" s="2" t="n">
+      <c r="D123" s="1" t="n">
         <v>43905</v>
       </c>
     </row>
-    <row r="124" spans="1:12">
+    <row r="124" spans="1:4">
       <c r="A124" t="n">
         <v>185</v>
       </c>
@@ -2490,11 +2487,11 @@
       <c r="C124" t="s">
         <v>6</v>
       </c>
-      <c r="D124" s="2" t="n">
+      <c r="D124" s="1" t="n">
         <v>43905</v>
       </c>
     </row>
-    <row r="125" spans="1:12">
+    <row r="125" spans="1:4">
       <c r="A125" t="n">
         <v>204</v>
       </c>
@@ -2504,11 +2501,11 @@
       <c r="C125" t="s">
         <v>23</v>
       </c>
-      <c r="D125" s="2" t="n">
+      <c r="D125" s="1" t="n">
         <v>43905</v>
       </c>
     </row>
-    <row r="126" spans="1:11">
+    <row r="126" spans="1:4">
       <c r="A126" t="n">
         <v>206</v>
       </c>
@@ -2518,11 +2515,11 @@
       <c r="C126" t="s">
         <v>15</v>
       </c>
-      <c r="D126" s="2" t="n">
+      <c r="D126" s="1" t="n">
         <v>43905</v>
       </c>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:4">
       <c r="A127" t="n">
         <v>207</v>
       </c>
@@ -2532,11 +2529,11 @@
       <c r="C127" t="s">
         <v>15</v>
       </c>
-      <c r="D127" s="2" t="n">
+      <c r="D127" s="1" t="n">
         <v>43905</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:4">
       <c r="A128" t="n">
         <v>224</v>
       </c>
@@ -2546,7 +2543,7 @@
       <c r="C128" t="s">
         <v>15</v>
       </c>
-      <c r="D128" s="2" t="n">
+      <c r="D128" s="1" t="n">
         <v>43905</v>
       </c>
     </row>
@@ -2560,7 +2557,7 @@
       <c r="C129" t="s">
         <v>15</v>
       </c>
-      <c r="D129" s="2" t="n">
+      <c r="D129" s="1" t="n">
         <v>43905</v>
       </c>
     </row>
@@ -2574,14 +2571,14 @@
       <c r="C130" t="s">
         <v>6</v>
       </c>
-      <c r="D130" s="2" t="n">
+      <c r="D130" s="1" t="n">
         <v>43906</v>
       </c>
       <c r="E130" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:4">
       <c r="A131" t="n">
         <v>64</v>
       </c>
@@ -2591,11 +2588,11 @@
       <c r="C131" t="s">
         <v>15</v>
       </c>
-      <c r="D131" s="2" t="n">
+      <c r="D131" s="1" t="n">
         <v>43906</v>
       </c>
     </row>
-    <row r="132" spans="1:12">
+    <row r="132" spans="1:4">
       <c r="A132" t="n">
         <v>66</v>
       </c>
@@ -2605,11 +2602,11 @@
       <c r="C132" t="s">
         <v>15</v>
       </c>
-      <c r="D132" s="2" t="n">
+      <c r="D132" s="1" t="n">
         <v>43906</v>
       </c>
     </row>
-    <row r="133" spans="1:12">
+    <row r="133" spans="1:5">
       <c r="A133" t="n">
         <v>70</v>
       </c>
@@ -2619,14 +2616,14 @@
       <c r="C133" t="s">
         <v>6</v>
       </c>
-      <c r="D133" s="2" t="n">
+      <c r="D133" s="1" t="n">
         <v>43906</v>
       </c>
       <c r="E133" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="134" spans="1:11">
+    <row r="134" spans="1:5">
       <c r="A134" t="n">
         <v>71</v>
       </c>
@@ -2636,14 +2633,14 @@
       <c r="C134" t="s">
         <v>6</v>
       </c>
-      <c r="D134" s="2" t="n">
+      <c r="D134" s="1" t="n">
         <v>43906</v>
       </c>
       <c r="E134" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:4">
       <c r="A135" t="n">
         <v>74</v>
       </c>
@@ -2653,7 +2650,7 @@
       <c r="C135" t="s">
         <v>23</v>
       </c>
-      <c r="D135" s="2" t="n">
+      <c r="D135" s="1" t="n">
         <v>43906</v>
       </c>
     </row>
@@ -2667,7 +2664,7 @@
       <c r="C136" t="s">
         <v>15</v>
       </c>
-      <c r="D136" s="2" t="n">
+      <c r="D136" s="1" t="n">
         <v>43906</v>
       </c>
     </row>
@@ -2681,7 +2678,7 @@
       <c r="C137" t="s">
         <v>6</v>
       </c>
-      <c r="D137" s="2" t="n">
+      <c r="D137" s="1" t="n">
         <v>43906</v>
       </c>
     </row>
@@ -2695,7 +2692,7 @@
       <c r="C138" t="s">
         <v>42</v>
       </c>
-      <c r="D138" s="2" t="n">
+      <c r="D138" s="1" t="n">
         <v>43906</v>
       </c>
     </row>
@@ -2709,7 +2706,7 @@
       <c r="C139" t="s">
         <v>6</v>
       </c>
-      <c r="D139" s="2" t="n">
+      <c r="D139" s="1" t="n">
         <v>43906</v>
       </c>
       <c r="E139" t="s">
@@ -2719,7 +2716,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:5">
       <c r="A140" t="n">
         <v>77</v>
       </c>
@@ -2729,7 +2726,7 @@
       <c r="C140" t="s">
         <v>6</v>
       </c>
-      <c r="D140" s="2" t="n">
+      <c r="D140" s="1" t="n">
         <v>43907</v>
       </c>
       <c r="E140" t="s">
@@ -2746,14 +2743,14 @@
       <c r="C141" t="s">
         <v>6</v>
       </c>
-      <c r="D141" s="2" t="n">
+      <c r="D141" s="1" t="n">
         <v>43907</v>
       </c>
       <c r="E141" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:4">
       <c r="A142" t="n">
         <v>89</v>
       </c>
@@ -2763,7 +2760,7 @@
       <c r="C142" t="s">
         <v>15</v>
       </c>
-      <c r="D142" s="2" t="n">
+      <c r="D142" s="1" t="n">
         <v>43907</v>
       </c>
     </row>
@@ -2777,7 +2774,7 @@
       <c r="C143" t="s">
         <v>45</v>
       </c>
-      <c r="D143" s="2" t="n">
+      <c r="D143" s="1" t="n">
         <v>43907</v>
       </c>
     </row>
@@ -2791,7 +2788,7 @@
       <c r="C144" t="s">
         <v>46</v>
       </c>
-      <c r="D144" s="2" t="n">
+      <c r="D144" s="1" t="n">
         <v>43907</v>
       </c>
     </row>
@@ -2805,7 +2802,7 @@
       <c r="C145" t="s">
         <v>6</v>
       </c>
-      <c r="D145" s="2" t="n">
+      <c r="D145" s="1" t="n">
         <v>43907</v>
       </c>
       <c r="E145" t="s">
@@ -2815,7 +2812,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="146" spans="1:12">
+    <row r="146" spans="1:6">
       <c r="A146" t="n">
         <v>162</v>
       </c>
@@ -2825,7 +2822,7 @@
       <c r="C146" t="s">
         <v>42</v>
       </c>
-      <c r="D146" s="2" t="n">
+      <c r="D146" s="1" t="n">
         <v>43907</v>
       </c>
       <c r="E146" t="s">
@@ -2835,7 +2832,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="147" spans="1:12">
+    <row r="147" spans="1:6">
       <c r="A147" t="n">
         <v>163</v>
       </c>
@@ -2845,7 +2842,7 @@
       <c r="C147" t="s">
         <v>6</v>
       </c>
-      <c r="D147" s="2" t="n">
+      <c r="D147" s="1" t="n">
         <v>43907</v>
       </c>
       <c r="E147" t="s">
@@ -2855,7 +2852,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="148" spans="1:12">
+    <row r="148" spans="1:4">
       <c r="A148" t="n">
         <v>203</v>
       </c>
@@ -2865,11 +2862,11 @@
       <c r="C148" t="s">
         <v>15</v>
       </c>
-      <c r="D148" s="2" t="n">
+      <c r="D148" s="1" t="n">
         <v>43907</v>
       </c>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:4">
       <c r="A149" t="n">
         <v>220</v>
       </c>
@@ -2879,11 +2876,11 @@
       <c r="C149" t="s">
         <v>23</v>
       </c>
-      <c r="D149" s="2" t="n">
+      <c r="D149" s="1" t="n">
         <v>43907</v>
       </c>
     </row>
-    <row r="150" spans="1:12">
+    <row r="150" spans="1:4">
       <c r="A150" t="n">
         <v>234</v>
       </c>
@@ -2893,7 +2890,7 @@
       <c r="C150" t="s">
         <v>23</v>
       </c>
-      <c r="D150" s="2" t="n">
+      <c r="D150" s="1" t="n">
         <v>43907</v>
       </c>
     </row>
@@ -2907,14 +2904,14 @@
       <c r="C151" t="s">
         <v>6</v>
       </c>
-      <c r="D151" s="2" t="n">
+      <c r="D151" s="1" t="n">
         <v>43908</v>
       </c>
       <c r="E151" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="152" spans="1:11">
+    <row r="152" spans="1:5">
       <c r="A152" t="n">
         <v>85</v>
       </c>
@@ -2924,14 +2921,14 @@
       <c r="C152" t="s">
         <v>6</v>
       </c>
-      <c r="D152" s="2" t="n">
+      <c r="D152" s="1" t="n">
         <v>43908</v>
       </c>
       <c r="E152" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:11">
+    <row r="153" spans="1:5">
       <c r="A153" t="n">
         <v>93</v>
       </c>
@@ -2941,14 +2938,14 @@
       <c r="C153" t="s">
         <v>6</v>
       </c>
-      <c r="D153" s="2" t="n">
+      <c r="D153" s="1" t="n">
         <v>43908</v>
       </c>
       <c r="E153" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="154" spans="1:11">
+    <row r="154" spans="1:4">
       <c r="A154" t="n">
         <v>94</v>
       </c>
@@ -2958,11 +2955,11 @@
       <c r="C154" t="s">
         <v>48</v>
       </c>
-      <c r="D154" s="2" t="n">
+      <c r="D154" s="1" t="n">
         <v>43908</v>
       </c>
     </row>
-    <row r="155" spans="1:11">
+    <row r="155" spans="1:4">
       <c r="A155" t="n">
         <v>95</v>
       </c>
@@ -2972,7 +2969,7 @@
       <c r="C155" t="s">
         <v>15</v>
       </c>
-      <c r="D155" s="2" t="n">
+      <c r="D155" s="1" t="n">
         <v>43908</v>
       </c>
     </row>
@@ -2986,11 +2983,11 @@
       <c r="C156" t="s">
         <v>15</v>
       </c>
-      <c r="D156" s="2" t="n">
+      <c r="D156" s="1" t="n">
         <v>43908</v>
       </c>
     </row>
-    <row r="157" spans="1:11">
+    <row r="157" spans="1:4">
       <c r="A157" t="n">
         <v>101</v>
       </c>
@@ -3000,11 +2997,11 @@
       <c r="C157" t="s">
         <v>23</v>
       </c>
-      <c r="D157" s="2" t="n">
+      <c r="D157" s="1" t="n">
         <v>43908</v>
       </c>
     </row>
-    <row r="158" spans="1:11">
+    <row r="158" spans="1:5">
       <c r="A158" t="n">
         <v>102</v>
       </c>
@@ -3014,14 +3011,14 @@
       <c r="C158" t="s">
         <v>23</v>
       </c>
-      <c r="D158" s="2" t="n">
+      <c r="D158" s="1" t="n">
         <v>43908</v>
       </c>
       <c r="E158" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="159" spans="1:11">
+    <row r="159" spans="1:4">
       <c r="A159" t="n">
         <v>103</v>
       </c>
@@ -3031,11 +3028,11 @@
       <c r="C159" t="s">
         <v>23</v>
       </c>
-      <c r="D159" s="2" t="n">
+      <c r="D159" s="1" t="n">
         <v>43908</v>
       </c>
     </row>
-    <row r="160" spans="1:11">
+    <row r="160" spans="1:4">
       <c r="A160" t="n">
         <v>104</v>
       </c>
@@ -3045,11 +3042,11 @@
       <c r="C160" t="s">
         <v>23</v>
       </c>
-      <c r="D160" s="2" t="n">
+      <c r="D160" s="1" t="n">
         <v>43908</v>
       </c>
     </row>
-    <row r="161" spans="1:11">
+    <row r="161" spans="1:4">
       <c r="A161" t="n">
         <v>105</v>
       </c>
@@ -3059,11 +3056,11 @@
       <c r="C161" t="s">
         <v>23</v>
       </c>
-      <c r="D161" s="2" t="n">
+      <c r="D161" s="1" t="n">
         <v>43908</v>
       </c>
     </row>
-    <row r="162" spans="1:11">
+    <row r="162" spans="1:4">
       <c r="A162" t="n">
         <v>106</v>
       </c>
@@ -3073,11 +3070,11 @@
       <c r="C162" t="s">
         <v>23</v>
       </c>
-      <c r="D162" s="2" t="n">
+      <c r="D162" s="1" t="n">
         <v>43908</v>
       </c>
     </row>
-    <row r="163" spans="1:11">
+    <row r="163" spans="1:5">
       <c r="A163" t="n">
         <v>108</v>
       </c>
@@ -3087,14 +3084,14 @@
       <c r="C163" t="s">
         <v>23</v>
       </c>
-      <c r="D163" s="2" t="n">
+      <c r="D163" s="1" t="n">
         <v>43908</v>
       </c>
       <c r="E163" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="164" spans="1:12">
+    <row r="164" spans="1:5">
       <c r="A164" t="n">
         <v>112</v>
       </c>
@@ -3104,14 +3101,14 @@
       <c r="C164" t="s">
         <v>23</v>
       </c>
-      <c r="D164" s="2" t="n">
+      <c r="D164" s="1" t="n">
         <v>43908</v>
       </c>
       <c r="E164" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="165" spans="1:12">
+    <row r="165" spans="1:5">
       <c r="A165" t="n">
         <v>113</v>
       </c>
@@ -3121,14 +3118,14 @@
       <c r="C165" t="s">
         <v>23</v>
       </c>
-      <c r="D165" s="2" t="n">
+      <c r="D165" s="1" t="n">
         <v>43908</v>
       </c>
       <c r="E165" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="166" spans="1:11">
+    <row r="166" spans="1:4">
       <c r="A166" t="n">
         <v>115</v>
       </c>
@@ -3138,11 +3135,11 @@
       <c r="C166" t="s">
         <v>23</v>
       </c>
-      <c r="D166" s="2" t="n">
+      <c r="D166" s="1" t="n">
         <v>43908</v>
       </c>
     </row>
-    <row r="167" spans="1:11">
+    <row r="167" spans="1:4">
       <c r="A167" t="n">
         <v>121</v>
       </c>
@@ -3152,11 +3149,11 @@
       <c r="C167" t="s">
         <v>23</v>
       </c>
-      <c r="D167" s="2" t="n">
+      <c r="D167" s="1" t="n">
         <v>43908</v>
       </c>
     </row>
-    <row r="168" spans="1:12">
+    <row r="168" spans="1:4">
       <c r="A168" t="n">
         <v>134</v>
       </c>
@@ -3166,11 +3163,11 @@
       <c r="C168" t="s">
         <v>23</v>
       </c>
-      <c r="D168" s="2" t="n">
+      <c r="D168" s="1" t="n">
         <v>43908</v>
       </c>
     </row>
-    <row r="169" spans="1:11">
+    <row r="169" spans="1:4">
       <c r="A169" t="n">
         <v>179</v>
       </c>
@@ -3180,11 +3177,11 @@
       <c r="C169" t="s">
         <v>23</v>
       </c>
-      <c r="D169" s="2" t="n">
+      <c r="D169" s="1" t="n">
         <v>43908</v>
       </c>
     </row>
-    <row r="170" spans="1:12">
+    <row r="170" spans="1:6">
       <c r="A170" t="n">
         <v>209</v>
       </c>
@@ -3194,7 +3191,7 @@
       <c r="C170" t="s">
         <v>6</v>
       </c>
-      <c r="D170" s="2" t="n">
+      <c r="D170" s="1" t="n">
         <v>43908</v>
       </c>
       <c r="E170" t="s">
@@ -3204,7 +3201,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="171" spans="1:6">
+    <row r="171" spans="1:4">
       <c r="A171" t="n">
         <v>96</v>
       </c>
@@ -3214,11 +3211,11 @@
       <c r="C171" t="s">
         <v>15</v>
       </c>
-      <c r="D171" s="2" t="n">
+      <c r="D171" s="1" t="n">
         <v>43909</v>
       </c>
     </row>
-    <row r="172" spans="1:12">
+    <row r="172" spans="1:5">
       <c r="A172" t="n">
         <v>110</v>
       </c>
@@ -3228,14 +3225,14 @@
       <c r="C172" t="s">
         <v>23</v>
       </c>
-      <c r="D172" s="2" t="n">
+      <c r="D172" s="1" t="n">
         <v>43909</v>
       </c>
       <c r="E172" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="173" spans="1:12">
+    <row r="173" spans="1:5">
       <c r="A173" t="n">
         <v>111</v>
       </c>
@@ -3245,14 +3242,14 @@
       <c r="C173" t="s">
         <v>23</v>
       </c>
-      <c r="D173" s="2" t="n">
+      <c r="D173" s="1" t="n">
         <v>43909</v>
       </c>
       <c r="E173" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="174" spans="1:11">
+    <row r="174" spans="1:5">
       <c r="A174" t="n">
         <v>116</v>
       </c>
@@ -3262,14 +3259,14 @@
       <c r="C174" t="s">
         <v>6</v>
       </c>
-      <c r="D174" s="2" t="n">
+      <c r="D174" s="1" t="n">
         <v>43909</v>
       </c>
       <c r="E174" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="175" spans="1:11">
+    <row r="175" spans="1:5">
       <c r="A175" t="n">
         <v>117</v>
       </c>
@@ -3279,14 +3276,14 @@
       <c r="C175" t="s">
         <v>23</v>
       </c>
-      <c r="D175" s="2" t="n">
+      <c r="D175" s="1" t="n">
         <v>43909</v>
       </c>
       <c r="E175" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="176" spans="1:11">
+    <row r="176" spans="1:4">
       <c r="A176" t="n">
         <v>118</v>
       </c>
@@ -3296,11 +3293,11 @@
       <c r="C176" t="s">
         <v>23</v>
       </c>
-      <c r="D176" s="2" t="n">
+      <c r="D176" s="1" t="n">
         <v>43909</v>
       </c>
     </row>
-    <row r="177" spans="1:11">
+    <row r="177" spans="1:4">
       <c r="A177" t="n">
         <v>141</v>
       </c>
@@ -3310,11 +3307,11 @@
       <c r="C177" t="s">
         <v>6</v>
       </c>
-      <c r="D177" s="2" t="n">
+      <c r="D177" s="1" t="n">
         <v>43909</v>
       </c>
     </row>
-    <row r="178" spans="1:11">
+    <row r="178" spans="1:4">
       <c r="A178" t="n">
         <v>122</v>
       </c>
@@ -3324,11 +3321,11 @@
       <c r="C178" t="s">
         <v>51</v>
       </c>
-      <c r="D178" s="2" t="n">
+      <c r="D178" s="1" t="n">
         <v>43910</v>
       </c>
     </row>
-    <row r="179" spans="1:11">
+    <row r="179" spans="1:4">
       <c r="A179" t="n">
         <v>128</v>
       </c>
@@ -3338,11 +3335,11 @@
       <c r="C179" t="s">
         <v>23</v>
       </c>
-      <c r="D179" s="2" t="n">
+      <c r="D179" s="1" t="n">
         <v>43910</v>
       </c>
     </row>
-    <row r="180" spans="1:11">
+    <row r="180" spans="1:5">
       <c r="A180" t="n">
         <v>129</v>
       </c>
@@ -3352,14 +3349,14 @@
       <c r="C180" t="s">
         <v>23</v>
       </c>
-      <c r="D180" s="2" t="n">
+      <c r="D180" s="1" t="n">
         <v>43910</v>
       </c>
       <c r="E180" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:11">
+    <row r="181" spans="1:4">
       <c r="A181" t="n">
         <v>146</v>
       </c>
@@ -3369,11 +3366,11 @@
       <c r="C181" t="s">
         <v>23</v>
       </c>
-      <c r="D181" s="2" t="n">
+      <c r="D181" s="1" t="n">
         <v>43910</v>
       </c>
     </row>
-    <row r="182" spans="1:12">
+    <row r="182" spans="1:4">
       <c r="A182" t="n">
         <v>166</v>
       </c>
@@ -3383,11 +3380,11 @@
       <c r="C182" t="s">
         <v>23</v>
       </c>
-      <c r="D182" s="2" t="n">
+      <c r="D182" s="1" t="n">
         <v>43910</v>
       </c>
     </row>
-    <row r="183" spans="1:11">
+    <row r="183" spans="1:5">
       <c r="A183" t="n">
         <v>170</v>
       </c>
@@ -3397,14 +3394,14 @@
       <c r="C183" t="s">
         <v>6</v>
       </c>
-      <c r="D183" s="2" t="n">
+      <c r="D183" s="1" t="n">
         <v>43910</v>
       </c>
       <c r="E183" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="184" spans="1:11">
+    <row r="184" spans="1:5">
       <c r="A184" t="n">
         <v>180</v>
       </c>
@@ -3414,14 +3411,14 @@
       <c r="C184" t="s">
         <v>23</v>
       </c>
-      <c r="D184" s="2" t="n">
+      <c r="D184" s="1" t="n">
         <v>43910</v>
       </c>
       <c r="E184" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="185" spans="1:11">
+    <row r="185" spans="1:5">
       <c r="A185" t="n">
         <v>181</v>
       </c>
@@ -3431,14 +3428,14 @@
       <c r="C185" t="s">
         <v>23</v>
       </c>
-      <c r="D185" s="2" t="n">
+      <c r="D185" s="1" t="n">
         <v>43910</v>
       </c>
       <c r="E185" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="186" spans="1:11">
+    <row r="186" spans="1:5">
       <c r="A186" t="n">
         <v>182</v>
       </c>
@@ -3448,14 +3445,14 @@
       <c r="C186" t="s">
         <v>23</v>
       </c>
-      <c r="D186" s="2" t="n">
+      <c r="D186" s="1" t="n">
         <v>43910</v>
       </c>
       <c r="E186" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="187" spans="1:11">
+    <row r="187" spans="1:4">
       <c r="A187" t="n">
         <v>210</v>
       </c>
@@ -3465,7 +3462,7 @@
       <c r="C187" t="s">
         <v>23</v>
       </c>
-      <c r="D187" s="2" t="n">
+      <c r="D187" s="1" t="n">
         <v>43910</v>
       </c>
     </row>
@@ -3479,7 +3476,7 @@
       <c r="C188" t="s">
         <v>23</v>
       </c>
-      <c r="D188" s="2" t="n">
+      <c r="D188" s="1" t="n">
         <v>43910</v>
       </c>
       <c r="E188" t="s">
@@ -3496,7 +3493,7 @@
       <c r="C189" t="s">
         <v>23</v>
       </c>
-      <c r="D189" s="2" t="n">
+      <c r="D189" s="1" t="n">
         <v>43910</v>
       </c>
       <c r="E189" t="s">
@@ -3506,7 +3503,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="190" spans="1:11">
+    <row r="190" spans="1:5">
       <c r="A190" t="n">
         <v>228</v>
       </c>
@@ -3516,14 +3513,14 @@
       <c r="C190" t="s">
         <v>23</v>
       </c>
-      <c r="D190" s="2" t="n">
+      <c r="D190" s="1" t="n">
         <v>43910</v>
       </c>
       <c r="E190" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
+    <row r="191" spans="1:4">
       <c r="A191" t="n">
         <v>229</v>
       </c>
@@ -3533,7 +3530,7 @@
       <c r="C191" t="s">
         <v>23</v>
       </c>
-      <c r="D191" s="2" t="n">
+      <c r="D191" s="1" t="n">
         <v>43910</v>
       </c>
     </row>
@@ -3547,11 +3544,11 @@
       <c r="C192" t="s">
         <v>23</v>
       </c>
-      <c r="D192" s="2" t="n">
+      <c r="D192" s="1" t="n">
         <v>43910</v>
       </c>
     </row>
-    <row r="193" spans="1:11">
+    <row r="193" spans="1:4">
       <c r="A193" t="n">
         <v>238</v>
       </c>
@@ -3561,11 +3558,11 @@
       <c r="C193" t="s">
         <v>23</v>
       </c>
-      <c r="D193" s="2" t="n">
+      <c r="D193" s="1" t="n">
         <v>43910</v>
       </c>
     </row>
-    <row r="194" spans="1:12">
+    <row r="194" spans="1:4">
       <c r="A194" t="n">
         <v>240</v>
       </c>
@@ -3575,11 +3572,11 @@
       <c r="C194" t="s">
         <v>23</v>
       </c>
-      <c r="D194" s="2" t="n">
+      <c r="D194" s="1" t="n">
         <v>43910</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
+    <row r="195" spans="1:4">
       <c r="A195" t="n">
         <v>251</v>
       </c>
@@ -3593,7 +3590,7 @@
         <v>43910</v>
       </c>
     </row>
-    <row r="196" spans="1:12">
+    <row r="196" spans="1:4">
       <c r="A196" t="n">
         <v>257</v>
       </c>
@@ -3607,7 +3604,7 @@
         <v>43910</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
+    <row r="197" spans="1:4">
       <c r="A197" t="n">
         <v>258</v>
       </c>
@@ -3621,7 +3618,7 @@
         <v>43910</v>
       </c>
     </row>
-    <row r="198" spans="1:12">
+    <row r="198" spans="1:4">
       <c r="A198" t="n">
         <v>135</v>
       </c>
@@ -3631,11 +3628,11 @@
       <c r="C198" t="s">
         <v>23</v>
       </c>
-      <c r="D198" s="2" t="n">
+      <c r="D198" s="1" t="n">
         <v>43911</v>
       </c>
     </row>
-    <row r="199" spans="1:11">
+    <row r="199" spans="1:5">
       <c r="A199" t="n">
         <v>138</v>
       </c>
@@ -3645,14 +3642,14 @@
       <c r="C199" t="s">
         <v>23</v>
       </c>
-      <c r="D199" s="2" t="n">
+      <c r="D199" s="1" t="n">
         <v>43911</v>
       </c>
       <c r="E199" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="200" spans="1:12">
+    <row r="200" spans="1:5">
       <c r="A200" t="n">
         <v>139</v>
       </c>
@@ -3662,7 +3659,7 @@
       <c r="C200" t="s">
         <v>23</v>
       </c>
-      <c r="D200" s="2" t="n">
+      <c r="D200" s="1" t="n">
         <v>43911</v>
       </c>
       <c r="E200" t="s">
@@ -3679,7 +3676,7 @@
       <c r="C201" t="s">
         <v>23</v>
       </c>
-      <c r="D201" s="2" t="n">
+      <c r="D201" s="1" t="n">
         <v>43911</v>
       </c>
       <c r="E201" t="s">
@@ -3696,14 +3693,14 @@
       <c r="C202" t="s">
         <v>23</v>
       </c>
-      <c r="D202" s="2" t="n">
+      <c r="D202" s="1" t="n">
         <v>43911</v>
       </c>
       <c r="E202" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
+    <row r="203" spans="1:4">
       <c r="A203" t="n">
         <v>147</v>
       </c>
@@ -3713,11 +3710,11 @@
       <c r="C203" t="s">
         <v>23</v>
       </c>
-      <c r="D203" s="2" t="n">
+      <c r="D203" s="1" t="n">
         <v>43911</v>
       </c>
     </row>
-    <row r="204" spans="1:11">
+    <row r="204" spans="1:4">
       <c r="A204" t="n">
         <v>153</v>
       </c>
@@ -3727,11 +3724,11 @@
       <c r="C204" t="s">
         <v>23</v>
       </c>
-      <c r="D204" s="2" t="n">
+      <c r="D204" s="1" t="n">
         <v>43911</v>
       </c>
     </row>
-    <row r="205" spans="1:11">
+    <row r="205" spans="1:4">
       <c r="A205" t="n">
         <v>241</v>
       </c>
@@ -3741,11 +3738,11 @@
       <c r="C205" t="s">
         <v>23</v>
       </c>
-      <c r="D205" s="2" t="n">
+      <c r="D205" s="1" t="n">
         <v>43911</v>
       </c>
     </row>
-    <row r="206" spans="1:11">
+    <row r="206" spans="1:4">
       <c r="A206" t="n">
         <v>130</v>
       </c>
@@ -3755,11 +3752,11 @@
       <c r="C206" t="s">
         <v>23</v>
       </c>
-      <c r="D206" s="2" t="n">
+      <c r="D206" s="1" t="n">
         <v>43912</v>
       </c>
     </row>
-    <row r="207" spans="1:12">
+    <row r="207" spans="1:4">
       <c r="A207" t="n">
         <v>131</v>
       </c>
@@ -3769,7 +3766,7 @@
       <c r="C207" t="s">
         <v>23</v>
       </c>
-      <c r="D207" s="2" t="n">
+      <c r="D207" s="1" t="n">
         <v>43912</v>
       </c>
     </row>
@@ -3783,7 +3780,7 @@
       <c r="C208" t="s">
         <v>23</v>
       </c>
-      <c r="D208" s="2" t="n">
+      <c r="D208" s="1" t="n">
         <v>43912</v>
       </c>
       <c r="E208" t="s">
@@ -3793,7 +3790,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="209" spans="1:6">
+    <row r="209" spans="1:4">
       <c r="A209" t="n">
         <v>133</v>
       </c>
@@ -3803,7 +3800,7 @@
       <c r="C209" t="s">
         <v>56</v>
       </c>
-      <c r="D209" s="2" t="n">
+      <c r="D209" s="1" t="n">
         <v>43912</v>
       </c>
     </row>
@@ -3817,11 +3814,11 @@
       <c r="C210" t="s">
         <v>23</v>
       </c>
-      <c r="D210" s="2" t="n">
+      <c r="D210" s="1" t="n">
         <v>43912</v>
       </c>
     </row>
-    <row r="211" spans="1:6">
+    <row r="211" spans="1:4">
       <c r="A211" t="n">
         <v>145</v>
       </c>
@@ -3831,11 +3828,11 @@
       <c r="C211" t="s">
         <v>23</v>
       </c>
-      <c r="D211" s="2" t="n">
+      <c r="D211" s="1" t="n">
         <v>43912</v>
       </c>
     </row>
-    <row r="212" spans="1:12">
+    <row r="212" spans="1:4">
       <c r="A212" t="n">
         <v>154</v>
       </c>
@@ -3845,11 +3842,11 @@
       <c r="C212" t="s">
         <v>23</v>
       </c>
-      <c r="D212" s="2" t="n">
+      <c r="D212" s="1" t="n">
         <v>43912</v>
       </c>
     </row>
-    <row r="213" spans="1:5">
+    <row r="213" spans="1:4">
       <c r="A213" t="n">
         <v>155</v>
       </c>
@@ -3859,7 +3856,7 @@
       <c r="C213" t="s">
         <v>23</v>
       </c>
-      <c r="D213" s="2" t="n">
+      <c r="D213" s="1" t="n">
         <v>43912</v>
       </c>
     </row>
@@ -3873,11 +3870,11 @@
       <c r="C214" t="s">
         <v>23</v>
       </c>
-      <c r="D214" s="2" t="n">
+      <c r="D214" s="1" t="n">
         <v>43912</v>
       </c>
     </row>
-    <row r="215" spans="1:5">
+    <row r="215" spans="1:4">
       <c r="A215" t="n">
         <v>160</v>
       </c>
@@ -3887,11 +3884,11 @@
       <c r="C215" t="s">
         <v>23</v>
       </c>
-      <c r="D215" s="2" t="n">
+      <c r="D215" s="1" t="n">
         <v>43912</v>
       </c>
     </row>
-    <row r="216" spans="1:11">
+    <row r="216" spans="1:4">
       <c r="A216" t="n">
         <v>172</v>
       </c>
@@ -3901,7 +3898,7 @@
       <c r="C216" t="s">
         <v>56</v>
       </c>
-      <c r="D216" s="2" t="n">
+      <c r="D216" s="1" t="n">
         <v>43912</v>
       </c>
     </row>
@@ -3915,14 +3912,14 @@
       <c r="C217" t="s">
         <v>6</v>
       </c>
-      <c r="D217" s="2" t="n">
+      <c r="D217" s="1" t="n">
         <v>43912</v>
       </c>
       <c r="E217" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="218" spans="1:5">
+    <row r="218" spans="1:4">
       <c r="A218" t="n">
         <v>249</v>
       </c>
@@ -3932,7 +3929,7 @@
       <c r="C218" t="s">
         <v>23</v>
       </c>
-      <c r="D218" s="2" t="n">
+      <c r="D218" s="1" t="n">
         <v>43912</v>
       </c>
     </row>
@@ -3946,14 +3943,14 @@
       <c r="C219" t="s">
         <v>23</v>
       </c>
-      <c r="D219" s="2" t="n">
+      <c r="D219" s="1" t="n">
         <v>43913</v>
       </c>
       <c r="E219" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="220" spans="1:5">
+    <row r="220" spans="1:4">
       <c r="A220" t="n">
         <v>164</v>
       </c>
@@ -3963,7 +3960,7 @@
       <c r="C220" t="s">
         <v>23</v>
       </c>
-      <c r="D220" s="2" t="n">
+      <c r="D220" s="1" t="n">
         <v>43913</v>
       </c>
     </row>
@@ -3977,14 +3974,14 @@
       <c r="C221" t="s">
         <v>23</v>
       </c>
-      <c r="D221" s="2" t="n">
+      <c r="D221" s="1" t="n">
         <v>43913</v>
       </c>
       <c r="E221" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="222" spans="1:11">
+    <row r="222" spans="1:4">
       <c r="A222" t="n">
         <v>216</v>
       </c>
@@ -3994,7 +3991,7 @@
       <c r="C222" t="s">
         <v>23</v>
       </c>
-      <c r="D222" s="2" t="n">
+      <c r="D222" s="1" t="n">
         <v>43913</v>
       </c>
     </row>
@@ -4008,7 +4005,7 @@
       <c r="C223" t="s">
         <v>23</v>
       </c>
-      <c r="D223" s="2" t="n">
+      <c r="D223" s="1" t="n">
         <v>43913</v>
       </c>
     </row>
@@ -4022,7 +4019,7 @@
       <c r="C224" t="s">
         <v>23</v>
       </c>
-      <c r="D224" s="2" t="n">
+      <c r="D224" s="1" t="n">
         <v>43914</v>
       </c>
       <c r="E224" t="s">
@@ -4039,14 +4036,14 @@
       <c r="C225" t="s">
         <v>23</v>
       </c>
-      <c r="D225" s="2" t="n">
+      <c r="D225" s="1" t="n">
         <v>43915</v>
       </c>
       <c r="E225" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="226" spans="1:5">
+    <row r="226" spans="1:4">
       <c r="A226" t="n">
         <v>217</v>
       </c>
@@ -4056,11 +4053,11 @@
       <c r="C226" t="s">
         <v>23</v>
       </c>
-      <c r="D226" s="2" t="n">
+      <c r="D226" s="1" t="n">
         <v>43915</v>
       </c>
     </row>
-    <row r="227" spans="1:11">
+    <row r="227" spans="1:4">
       <c r="A227" t="n">
         <v>218</v>
       </c>
@@ -4070,11 +4067,11 @@
       <c r="C227" t="s">
         <v>23</v>
       </c>
-      <c r="D227" s="2" t="n">
+      <c r="D227" s="1" t="n">
         <v>43915</v>
       </c>
     </row>
-    <row r="228" spans="1:11">
+    <row r="228" spans="1:4">
       <c r="A228" t="n">
         <v>225</v>
       </c>
@@ -4084,11 +4081,11 @@
       <c r="C228" t="s">
         <v>23</v>
       </c>
-      <c r="D228" s="2" t="n">
+      <c r="D228" s="1" t="n">
         <v>43915</v>
       </c>
     </row>
-    <row r="229" spans="1:11">
+    <row r="229" spans="1:4">
       <c r="A229" t="n">
         <v>242</v>
       </c>
@@ -4098,11 +4095,11 @@
       <c r="C229" t="s">
         <v>23</v>
       </c>
-      <c r="D229" s="2" t="n">
+      <c r="D229" s="1" t="n">
         <v>43915</v>
       </c>
     </row>
-    <row r="230" spans="1:11">
+    <row r="230" spans="1:4">
       <c r="A230" t="n">
         <v>244</v>
       </c>
@@ -4112,11 +4109,11 @@
       <c r="C230" t="s">
         <v>23</v>
       </c>
-      <c r="D230" s="2" t="n">
+      <c r="D230" s="1" t="n">
         <v>43915</v>
       </c>
     </row>
-    <row r="231" spans="1:11">
+    <row r="231" spans="1:4">
       <c r="A231" t="n">
         <v>245</v>
       </c>
@@ -4126,7 +4123,7 @@
       <c r="C231" t="s">
         <v>23</v>
       </c>
-      <c r="D231" s="2" t="n">
+      <c r="D231" s="1" t="n">
         <v>43915</v>
       </c>
     </row>
@@ -4140,7 +4137,7 @@
       <c r="C232" t="s">
         <v>23</v>
       </c>
-      <c r="D232" s="2" t="n">
+      <c r="D232" s="1" t="n">
         <v>43915</v>
       </c>
     </row>
@@ -4154,11 +4151,11 @@
       <c r="C233" t="s">
         <v>23</v>
       </c>
-      <c r="D233" s="2" t="n">
+      <c r="D233" s="1" t="n">
         <v>43917</v>
       </c>
     </row>
-    <row r="234" spans="1:11">
+    <row r="234" spans="1:4">
       <c r="A234" t="n">
         <v>226</v>
       </c>
@@ -4168,11 +4165,11 @@
       <c r="C234" t="s">
         <v>23</v>
       </c>
-      <c r="D234" s="2" t="n">
+      <c r="D234" s="1" t="n">
         <v>43917</v>
       </c>
     </row>
-    <row r="235" spans="1:11">
+    <row r="235" spans="1:5">
       <c r="A235" t="n">
         <v>231</v>
       </c>
@@ -4182,14 +4179,14 @@
       <c r="C235" t="s">
         <v>54</v>
       </c>
-      <c r="D235" s="2" t="n">
+      <c r="D235" s="1" t="n">
         <v>43917</v>
       </c>
       <c r="E235" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="236" spans="1:5">
+    <row r="236" spans="1:4">
       <c r="A236" t="n">
         <v>232</v>
       </c>
@@ -4199,7 +4196,7 @@
       <c r="C236" t="s">
         <v>23</v>
       </c>
-      <c r="D236" s="2" t="n">
+      <c r="D236" s="1" t="n">
         <v>43917</v>
       </c>
     </row>
@@ -4213,11 +4210,11 @@
       <c r="C237" t="s">
         <v>23</v>
       </c>
-      <c r="D237" s="2" t="n">
+      <c r="D237" s="1" t="n">
         <v>43917</v>
       </c>
     </row>
-    <row r="238" spans="1:11">
+    <row r="238" spans="1:4">
       <c r="A238" t="n">
         <v>255</v>
       </c>
@@ -4231,7 +4228,7 @@
         <v>43917</v>
       </c>
     </row>
-    <row r="239" spans="1:11">
+    <row r="239" spans="1:4">
       <c r="A239" t="n">
         <v>256</v>
       </c>
@@ -4245,7 +4242,7 @@
         <v>43917</v>
       </c>
     </row>
-    <row r="240" spans="1:6">
+    <row r="240" spans="1:4">
       <c r="A240" t="n">
         <v>250</v>
       </c>
@@ -4269,11 +4266,11 @@
       <c r="C241" t="s">
         <v>15</v>
       </c>
-      <c r="D241" s="2" t="n">
-        <v>44047</v>
-      </c>
-    </row>
-    <row r="242" spans="1:11">
+      <c r="D241" s="1" t="n">
+        <v>43929</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4">
       <c r="A242" t="n">
         <v>253</v>
       </c>
@@ -4283,8 +4280,8 @@
       <c r="C242" t="s">
         <v>6</v>
       </c>
-      <c r="D242" s="2" t="n">
-        <v>44078</v>
+      <c r="D242" s="1" t="n">
+        <v>43930</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -4297,15 +4294,15 @@
       <c r="C243" t="s">
         <v>6</v>
       </c>
-      <c r="D243" s="2" t="n">
-        <v>44078</v>
+      <c r="D243" s="1" t="n">
+        <v>43930</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1586665606" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1586694348" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4314,16 +4311,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1586665606" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1586665606" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1586665606" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1586665606" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1586694348" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1586694348" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1586694348" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1586694348" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1586665606" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1586694348" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>